<commit_message>
2nd modify in excel
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10User\Desktop\coach rony\web 0\session8 deploy api &amp; install free template\api\items api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05DFAA1-C123-40DE-BC03-977E2D767185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269BEB39-33D4-4EEC-B857-21561122F6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>available</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>iphone 6</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>images</t>
   </si>
 </sst>
 </file>
@@ -236,8 +236,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -320,21 +320,17 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -620,38 +616,38 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="7" max="7" width="85.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -659,22 +655,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5">
         <v>50</v>
       </c>
-      <c r="D2" s="4">
-        <v>50</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -682,22 +678,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5">
         <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -705,22 +701,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5">
         <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -728,22 +724,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
         <v>160</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -751,22 +747,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5">
         <v>250</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -774,22 +770,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5">
         <v>500</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -797,22 +793,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5">
         <v>700</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -820,22 +816,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5">
         <v>1000</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -843,22 +839,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="4">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5">
         <v>130</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -866,22 +862,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="4">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5">
         <v>300</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -889,22 +885,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>125</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -912,22 +908,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="4">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5">
         <v>270</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -935,22 +931,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="4">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5">
         <v>430</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -958,22 +954,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="4">
+        <v>25</v>
+      </c>
+      <c r="D15" s="5">
         <v>300</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -981,22 +977,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="4">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5">
         <v>350</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1004,22 +1000,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5">
         <v>450</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1027,22 +1023,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="4">
+        <v>26</v>
+      </c>
+      <c r="D18" s="5">
         <v>390</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1050,22 +1046,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5">
         <v>450</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1073,22 +1069,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="D20" s="5">
         <v>400</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1096,22 +1092,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5">
         <v>360</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1119,22 +1115,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5">
+        <v>550</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="4">
-        <v>550</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1142,22 +1138,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="4">
+        <v>21</v>
+      </c>
+      <c r="D23" s="5">
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1165,22 +1161,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="D24" s="5">
         <v>1000</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1188,22 +1184,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="4">
+        <v>24</v>
+      </c>
+      <c r="D25" s="5">
         <v>890</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new items to excel
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10User\Desktop\coach rony\web 0\session8 deploy api &amp; install free template\api\items api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069F41BB-E363-4F1D-A7E9-EC125AED17E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D6851C-84F8-4519-A107-3AD3C56A6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -69,9 +69,6 @@
     <t>lg32</t>
   </si>
   <si>
-    <t>lg40</t>
-  </si>
-  <si>
     <t>refrigerator</t>
   </si>
   <si>
@@ -214,6 +211,24 @@
   </si>
   <si>
     <t>https://github.com/mostafaljamal85/imagesItems/blob/main/whirlpool.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>lg42</t>
+  </si>
+  <si>
+    <t>https://github.com/mostafaljamal85/imagesItems/blob/main/boshRef.png?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/mostafaljamal85/imagesItems/blob/main/campomaticRef.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/mostafaljamal85/imagesItems/blob/main/dellpc.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/mostafaljamal85/imagesItems/blob/main/lg42.jpg?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/mostafaljamal85/imagesItems/blob/main/samsungW.jpg?raw=true</t>
   </si>
 </sst>
 </file>
@@ -600,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10611ACE-F244-40E4-B38A-A02A4F93AFA8}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,10 +635,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -632,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -643,19 +658,19 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="5">
         <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -672,13 +687,13 @@
         <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -695,13 +710,13 @@
         <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -718,13 +733,13 @@
         <v>160</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -741,13 +756,13 @@
         <v>250</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -764,13 +779,13 @@
         <v>500</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -787,13 +802,13 @@
         <v>700</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -810,13 +825,13 @@
         <v>1000</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -827,19 +842,19 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5">
         <v>130</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -850,19 +865,19 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5">
         <v>300</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -879,13 +894,13 @@
         <v>125</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -896,18 +911,20 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5">
         <v>270</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
@@ -917,19 +934,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5">
         <v>430</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -937,43 +954,45 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5">
         <v>300</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5">
         <v>350</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -981,64 +1000,68 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D17" s="5">
         <v>450</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5">
         <v>390</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5">
         <v>450</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1046,22 +1069,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D20" s="5">
         <v>400</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1069,22 +1092,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="5">
         <v>360</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1092,22 +1115,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="5">
         <v>550</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1115,43 +1138,45 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="5">
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D24" s="5">
         <v>1000</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1159,22 +1184,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="5">
         <v>890</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit  features of items
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10User\Desktop\coach rony\web 0\session8 deploy api &amp; install free template\api\items api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDE5E40-9794-4593-BB99-EE7A3A47463B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A95913-7BC3-4A52-AA42-222278E64D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,12 +108,6 @@
     <t>lenovo</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>Available</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,21 +627,22 @@
     <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="85.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -650,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -661,19 +662,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5">
         <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -690,13 +691,13 @@
         <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -713,13 +714,13 @@
         <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -736,13 +737,13 @@
         <v>160</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -759,13 +760,13 @@
         <v>250</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -782,13 +783,13 @@
         <v>500</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -805,13 +806,13 @@
         <v>700</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -828,13 +829,13 @@
         <v>1000</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -845,19 +846,19 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5">
         <v>130</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -868,19 +869,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5">
         <v>300</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -897,13 +898,13 @@
         <v>125</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -914,19 +915,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="5">
         <v>270</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -937,19 +938,19 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="5">
         <v>430</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -966,13 +967,13 @@
         <v>300</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -983,19 +984,19 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5">
         <v>350</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1012,13 +1013,13 @@
         <v>450</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1035,13 +1036,13 @@
         <v>390</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1058,13 +1059,13 @@
         <v>450</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1081,13 +1082,13 @@
         <v>400</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1104,13 +1105,13 @@
         <v>360</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1127,13 +1128,13 @@
         <v>550</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1150,13 +1151,13 @@
         <v>600</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1173,13 +1174,13 @@
         <v>1000</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1196,13 +1197,13 @@
         <v>890</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>